<commit_message>
Reorganización de las carpetas
</commit_message>
<xml_diff>
--- a/0. Analisis/Calendario Entregas/Formato Seleccion Personal Wuki.xlsx
+++ b/0. Analisis/Calendario Entregas/Formato Seleccion Personal Wuki.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Nalsani S.A.S\Escritorio\proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaly\OneDrive\Documentos\GitHub\WebWuky\0. Analisis\Calendario Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FE7743D-B475-440F-A591-5009FBF6BA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12436B38-F6DB-4D26-A024-16428A751C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seleccion Personal" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -58,9 +71,6 @@
     <t>3006496800/ jgbenavides3@misena.edu.co</t>
   </si>
   <si>
-    <t>WUKI</t>
-  </si>
-  <si>
     <t>3022227547/paula.hernndez3@misena.edu.co</t>
   </si>
   <si>
@@ -80,6 +90,9 @@
   </si>
   <si>
     <t>Paula Hernandez</t>
+  </si>
+  <si>
+    <t>WUKY</t>
   </si>
 </sst>
 </file>
@@ -322,12 +335,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -438,9 +450,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,9 +490,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,26 +525,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -565,26 +560,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -760,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,44 +754,44 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
+      <c r="C5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="2:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -821,114 +799,114 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>16</v>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>18</v>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>14</v>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>